<commit_message>
#@Todd: The dimensions for quantity 'fraction.el.misclassified.ll' include 'continuum' and 'stage'. However these dimensions are not present in the outcome dim.names inferred from the other outcomes
</commit_message>
<xml_diff>
--- a/applications/SHIELD/support/contactTracing1.xlsx
+++ b/applications/SHIELD/support/contactTracing1.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="15" documentId="8_{B3072B77-8F0F-2842-9A51-5929F5064928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D91E798-2D1D-6742-9DF6-042295D4B653}"/>
   <bookViews>
-    <workbookView xWindow="73300" yWindow="720" windowWidth="37540" windowHeight="17440" xr2:uid="{B47A3F01-3C2A-774F-B5A4-9BB5BDC5E9A9}"/>
+    <workbookView xWindow="340" yWindow="720" windowWidth="37540" windowHeight="17440" xr2:uid="{B47A3F01-3C2A-774F-B5A4-9BB5BDC5E9A9}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -5793,7 +5793,7 @@
   <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:I48"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added misclassification error estimates for EL/LLU, and a prelim code to estiamte the variance of prenatal estimates at the MSA level
</commit_message>
<xml_diff>
--- a/applications/SHIELD/support/contactTracing1.xlsx
+++ b/applications/SHIELD/support/contactTracing1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/pkasaie1_jh_edu/Documents/SHIELDR01/Simulation/code/jheem_analyses/applications/SHIELD/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{B3072B77-8F0F-2842-9A51-5929F5064928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FAA22F0-58F7-1B4F-803A-0E1F08DDDD43}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{B3072B77-8F0F-2842-9A51-5929F5064928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{059BDC19-FD43-9943-BE0B-F4BA7BC7720A}"/>
   <bookViews>
     <workbookView xWindow="84240" yWindow="4760" windowWidth="34560" windowHeight="17440" activeTab="1" xr2:uid="{B47A3F01-3C2A-774F-B5A4-9BB5BDC5E9A9}"/>
   </bookViews>
@@ -7053,7 +7053,7 @@
   <dimension ref="E6:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
error with HIV testing cache object
</commit_message>
<xml_diff>
--- a/applications/SHIELD/support/contactTracing1.xlsx
+++ b/applications/SHIELD/support/contactTracing1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/pkasaie1_jh_edu/Documents/SHIELDR01/Simulation/code/jheem_analyses/applications/SHIELD/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{B3072B77-8F0F-2842-9A51-5929F5064928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{059BDC19-FD43-9943-BE0B-F4BA7BC7720A}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{B3072B77-8F0F-2842-9A51-5929F5064928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92532CF5-6CFD-3544-983D-B9954EC080D6}"/>
   <bookViews>
-    <workbookView xWindow="84240" yWindow="4760" windowWidth="34560" windowHeight="17440" activeTab="1" xr2:uid="{B47A3F01-3C2A-774F-B5A4-9BB5BDC5E9A9}"/>
+    <workbookView xWindow="49680" yWindow="5560" windowWidth="34560" windowHeight="17440" activeTab="1" xr2:uid="{B47A3F01-3C2A-774F-B5A4-9BB5BDC5E9A9}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -7053,7 +7053,7 @@
   <dimension ref="E6:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>